<commit_message>
Added images to slide book
</commit_message>
<xml_diff>
--- a/DBMVS.xlsx
+++ b/DBMVS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ut1169\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ut1169\Documents\my-virtual-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C190BE0B-83E9-4124-A49E-937AB2AD75BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A493067-9AC3-4079-98E8-320C66AE06BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B265EF8B-AD64-435F-AB1B-D90224CF4867}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B265EF8B-AD64-435F-AB1B-D90224CF4867}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>USER</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>STATES</t>
+  </si>
+  <si>
+    <t>IMAGES</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>FK 1 image -&gt; 1 o + user</t>
   </si>
 </sst>
 </file>
@@ -584,24 +593,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D9EEAF-A3E4-44F5-9B66-BCF638BCD3D5}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -614,10 +624,14 @@
         <v>52</v>
       </c>
       <c r="H1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -636,8 +650,14 @@
       <c r="H2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -656,16 +676,25 @@
       <c r="H3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
@@ -675,7 +704,7 @@
       </c>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -692,7 +721,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -842,7 +871,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>